<commit_message>
Added 3.1 - Simulation for complex strategies, with Stop Loss. Processed backtest and generated summaries for complex strategies
</commit_message>
<xml_diff>
--- a/Market_data.xlsx
+++ b/Market_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arek\Desktop\Praca magisterska\Praca magisterska SKRYPTY\In production\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arek\Desktop\Investment Strategies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6066C894-A6D6-4C88-9AEA-B6515969620B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6580FA3B-B7C6-48CF-AC3C-4BE8FCB4C8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="109">
   <si>
     <t>Ticker</t>
   </si>
   <si>
-    <t>Początek</t>
-  </si>
-  <si>
-    <t>Koniec</t>
-  </si>
-  <si>
     <t>Min. interwał</t>
   </si>
   <si>
-    <t>Plik</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -187,12 +178,6 @@
     <t>GSPC.INDX</t>
   </si>
   <si>
-    <t>INJ</t>
-  </si>
-  <si>
-    <t>INJUSDT</t>
-  </si>
-  <si>
     <t>JUP</t>
   </si>
   <si>
@@ -229,9 +214,6 @@
     <t>NDX.INDX</t>
   </si>
   <si>
-    <t>NVDA</t>
-  </si>
-  <si>
     <t>OM</t>
   </si>
   <si>
@@ -356,6 +338,15 @@
   </si>
   <si>
     <t>ZROUSDT</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
   </si>
 </sst>
 </file>
@@ -722,40 +713,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>43207</v>
@@ -764,21 +758,21 @@
         <v>45716</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>45667</v>
@@ -787,21 +781,21 @@
         <v>45716</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <v>44582</v>
@@ -810,21 +804,21 @@
         <v>45716</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2">
         <v>45008</v>
@@ -833,21 +827,21 @@
         <v>45716</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2">
         <v>44498</v>
@@ -856,21 +850,21 @@
         <v>45716</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>44096</v>
@@ -879,21 +873,21 @@
         <v>45716</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2">
         <v>45694</v>
@@ -902,21 +896,21 @@
         <v>45716</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2">
         <v>45275</v>
@@ -925,21 +919,21 @@
         <v>45716</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2">
         <v>42948</v>
@@ -948,21 +942,21 @@
         <v>45689</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2">
         <v>42360</v>
@@ -971,18 +965,18 @@
         <v>45716</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2">
         <v>42417</v>
@@ -991,18 +985,18 @@
         <v>45716</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2">
         <v>45667</v>
@@ -1011,21 +1005,21 @@
         <v>45716</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2">
         <v>43914</v>
@@ -1034,18 +1028,18 @@
         <v>45716</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2">
         <v>43651</v>
@@ -1054,21 +1048,21 @@
         <v>45716</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16" s="2">
         <v>45328</v>
@@ -1077,21 +1071,21 @@
         <v>45716</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2">
         <v>45566</v>
@@ -1100,21 +1094,21 @@
         <v>45716</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2">
         <v>45384</v>
@@ -1123,21 +1117,21 @@
         <v>45716</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2">
         <v>42964</v>
@@ -1146,21 +1140,21 @@
         <v>45716</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2">
         <v>40181</v>
@@ -1169,18 +1163,18 @@
         <v>45716</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2">
         <v>40181</v>
@@ -1189,18 +1183,18 @@
         <v>45716</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2">
         <v>43891</v>
@@ -1209,673 +1203,630 @@
         <v>45689</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B23" s="2">
-        <v>44125</v>
+        <v>45322</v>
       </c>
       <c r="C23" s="2">
         <v>45716</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B24" s="2">
-        <v>45322</v>
+        <v>45247</v>
       </c>
       <c r="C24" s="2">
         <v>45716</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B25" s="2">
-        <v>45247</v>
+        <v>43481</v>
       </c>
       <c r="C25" s="2">
         <v>45716</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B26" s="2">
-        <v>43481</v>
+        <v>43082</v>
       </c>
       <c r="C26" s="2">
         <v>45716</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B27" s="2">
-        <v>43082</v>
+        <v>40181</v>
       </c>
       <c r="C27" s="2">
         <v>45716</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>64</v>
-      </c>
-      <c r="F27" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="G27" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B28" s="2">
-        <v>40181</v>
+        <v>43914</v>
       </c>
       <c r="C28" s="2">
         <v>45716</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B29" s="2">
-        <v>43914</v>
+        <v>44263</v>
       </c>
       <c r="C29" s="2">
         <v>45716</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>68</v>
+        <v>65</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B30" s="2">
-        <v>40182</v>
+        <v>45051</v>
       </c>
       <c r="C30" s="2">
         <v>45716</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B31" s="2">
-        <v>44263</v>
+        <v>40182</v>
       </c>
       <c r="C31" s="2">
         <v>45716</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="G31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B32" s="2">
-        <v>45051</v>
+        <v>44104</v>
       </c>
       <c r="C32" s="2">
         <v>45716</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="G32" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B33" s="2">
-        <v>40182</v>
+        <v>45607</v>
       </c>
       <c r="C33" s="2">
         <v>45716</v>
       </c>
       <c r="D33" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="F33" t="s">
+        <v>7</v>
       </c>
       <c r="G33" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B34" s="2">
-        <v>44104</v>
+        <v>45324</v>
       </c>
       <c r="C34" s="2">
         <v>45716</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
       </c>
       <c r="G34" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B35" s="2">
-        <v>45607</v>
+        <v>45499</v>
       </c>
       <c r="C35" s="2">
         <v>45716</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F35" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G35" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B36" s="2">
-        <v>45324</v>
+        <v>44054</v>
       </c>
       <c r="C36" s="2">
         <v>45716</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F36" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G36" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B37" s="2">
-        <v>45499</v>
+        <v>45049</v>
       </c>
       <c r="C37" s="2">
         <v>45716</v>
       </c>
       <c r="D37" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F37" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G37" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B38" s="2">
-        <v>44054</v>
+        <v>45393</v>
       </c>
       <c r="C38" s="2">
         <v>45716</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F38" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G38" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B39" s="2">
-        <v>45049</v>
+        <v>45230</v>
       </c>
       <c r="C39" s="2">
         <v>45716</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F39" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B40" s="2">
-        <v>45393</v>
+        <v>45512</v>
       </c>
       <c r="C40" s="2">
         <v>45716</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F40" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B41" s="2">
-        <v>45230</v>
+        <v>45676</v>
       </c>
       <c r="C41" s="2">
         <v>45716</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G41" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B42" s="2">
-        <v>45512</v>
+        <v>43262</v>
       </c>
       <c r="C42" s="2">
         <v>45716</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F42" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G42" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B43" s="2">
-        <v>45676</v>
+        <v>40181</v>
       </c>
       <c r="C43" s="2">
         <v>45716</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E43" t="s">
-        <v>93</v>
-      </c>
-      <c r="F43" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="G43" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B44" s="2">
-        <v>43262</v>
+        <v>40179</v>
       </c>
       <c r="C44" s="2">
         <v>45716</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E44" t="s">
-        <v>95</v>
-      </c>
-      <c r="F44" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="G44" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B45" s="2">
-        <v>40181</v>
+        <v>45636</v>
       </c>
       <c r="C45" s="2">
         <v>45716</v>
       </c>
       <c r="D45" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
       </c>
       <c r="G45" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B46" s="2">
-        <v>40179</v>
+        <v>45131</v>
       </c>
       <c r="C46" s="2">
         <v>45716</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
       </c>
       <c r="G46" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B47" s="2">
-        <v>45636</v>
+        <v>40181</v>
       </c>
       <c r="C47" s="2">
         <v>45716</v>
       </c>
       <c r="D47" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E47" t="s">
-        <v>101</v>
-      </c>
-      <c r="F47" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="G47" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B48" s="2">
-        <v>45131</v>
+        <v>40181</v>
       </c>
       <c r="C48" s="2">
         <v>45716</v>
       </c>
       <c r="D48" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E48" t="s">
-        <v>103</v>
-      </c>
-      <c r="F48" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="G48" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B49" s="2">
-        <v>40181</v>
+        <v>40546</v>
       </c>
       <c r="C49" s="2">
         <v>45716</v>
       </c>
       <c r="D49" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G49" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B50" s="2">
-        <v>40181</v>
+        <v>45463</v>
       </c>
       <c r="C50" s="2">
         <v>45716</v>
       </c>
       <c r="D50" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
       </c>
       <c r="G50" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B51" s="2">
-        <v>40546</v>
-      </c>
-      <c r="C51" s="2">
-        <v>45716</v>
-      </c>
-      <c r="D51" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" t="s">
-        <v>109</v>
-      </c>
-      <c r="G51" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>110</v>
-      </c>
-      <c r="B52" s="2">
-        <v>45463</v>
-      </c>
-      <c r="C52" s="2">
-        <v>45716</v>
-      </c>
-      <c r="D52" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" t="s">
-        <v>111</v>
-      </c>
-      <c r="F52" t="s">
-        <v>10</v>
-      </c>
-      <c r="G52" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>